<commit_message>
FIX update of the main_building floor
</commit_message>
<xml_diff>
--- a/calculation/main_building_grid.xlsx
+++ b/calculation/main_building_grid.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="271">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -716,7 +716,7 @@
     <t xml:space="preserve">N Diagonalen_40 (d | m | m3)</t>
   </si>
   <si>
-    <t xml:space="preserve">72.75</t>
+    <t xml:space="preserve">80.13</t>
   </si>
   <si>
     <t xml:space="preserve">6.55</t>
@@ -734,6 +734,12 @@
     <t xml:space="preserve">14.08</t>
   </si>
   <si>
+    <t xml:space="preserve">13.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.31</t>
+  </si>
+  <si>
     <t xml:space="preserve">14.55</t>
   </si>
   <si>
@@ -743,6 +749,9 @@
     <t xml:space="preserve">14.78</t>
   </si>
   <si>
+    <t xml:space="preserve">15.25</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.42</t>
   </si>
   <si>
@@ -761,12 +770,6 @@
     <t xml:space="preserve">16.32</t>
   </si>
   <si>
-    <t xml:space="preserve">6.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.22</t>
-  </si>
-  <si>
     <t xml:space="preserve">13.9</t>
   </si>
   <si>
@@ -779,12 +782,18 @@
     <t xml:space="preserve">18.21</t>
   </si>
   <si>
+    <t xml:space="preserve">14.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">19.62</t>
   </si>
   <si>
     <t xml:space="preserve">14.03</t>
   </si>
   <si>
+    <t xml:space="preserve">21.48</t>
+  </si>
+  <si>
     <t xml:space="preserve">6.91</t>
   </si>
   <si>
@@ -807,6 +816,12 @@
   </si>
   <si>
     <t xml:space="preserve">17.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.3</t>
   </si>
   <si>
     <t xml:space="preserve">7.78</t>
@@ -925,7 +940,7 @@
         <v>158</v>
       </c>
       <c r="F3">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -1085,7 +1100,7 @@
         <v>179</v>
       </c>
       <c r="F11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12">
@@ -1105,7 +1120,7 @@
         <v>180</v>
       </c>
       <c r="F12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13">
@@ -1125,7 +1140,7 @@
         <v>177</v>
       </c>
       <c r="F13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14">
@@ -1145,7 +1160,7 @@
         <v>178</v>
       </c>
       <c r="F14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15">
@@ -1165,7 +1180,7 @@
         <v>179</v>
       </c>
       <c r="F15" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16">
@@ -1185,7 +1200,7 @@
         <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
@@ -1205,7 +1220,7 @@
         <v>181</v>
       </c>
       <c r="F17" t="s">
-        <v>120</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18">
@@ -1225,7 +1240,7 @@
         <v>182</v>
       </c>
       <c r="F18" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19">
@@ -1245,7 +1260,7 @@
         <v>183</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20">
@@ -1265,7 +1280,7 @@
         <v>184</v>
       </c>
       <c r="F20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21">
@@ -1305,7 +1320,7 @@
         <v>186</v>
       </c>
       <c r="F22" t="s">
-        <v>244</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23">
@@ -1325,7 +1340,7 @@
         <v>187</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24">
@@ -1345,7 +1360,7 @@
         <v>184</v>
       </c>
       <c r="F24" t="s">
-        <v>248</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
@@ -1405,7 +1420,7 @@
         <v>188</v>
       </c>
       <c r="F27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28">
@@ -1425,7 +1440,7 @@
         <v>189</v>
       </c>
       <c r="F28" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29">
@@ -1445,7 +1460,7 @@
         <v>185</v>
       </c>
       <c r="F29" t="s">
-        <v>252</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30">
@@ -1465,7 +1480,7 @@
         <v>186</v>
       </c>
       <c r="F30" t="s">
-        <v>250</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31">
@@ -1485,7 +1500,7 @@
         <v>188</v>
       </c>
       <c r="F31" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1540,7 @@
         <v>185</v>
       </c>
       <c r="F33" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34">
@@ -1545,7 +1560,7 @@
         <v>186</v>
       </c>
       <c r="F34" t="s">
-        <v>48</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35">
@@ -1565,7 +1580,7 @@
         <v>188</v>
       </c>
       <c r="F35" t="s">
-        <v>250</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
@@ -1585,7 +1600,7 @@
         <v>189</v>
       </c>
       <c r="F36" t="s">
-        <v>254</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37">
@@ -1605,7 +1620,7 @@
         <v>185</v>
       </c>
       <c r="F37" t="s">
-        <v>48</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38">
@@ -1625,7 +1640,7 @@
         <v>143</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39">
@@ -1665,7 +1680,7 @@
         <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41">
@@ -1685,7 +1700,7 @@
         <v>147</v>
       </c>
       <c r="F41" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42">
@@ -1705,7 +1720,7 @@
         <v>143</v>
       </c>
       <c r="F42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43">
@@ -1725,7 +1740,7 @@
         <v>147</v>
       </c>
       <c r="F43" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44">
@@ -1745,7 +1760,7 @@
         <v>190</v>
       </c>
       <c r="F44" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45">
@@ -1765,7 +1780,7 @@
         <v>147</v>
       </c>
       <c r="F45" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46">
@@ -1785,7 +1800,7 @@
         <v>143</v>
       </c>
       <c r="F46" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47">
@@ -1805,7 +1820,7 @@
         <v>147</v>
       </c>
       <c r="F47" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48">
@@ -1825,7 +1840,7 @@
         <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49">
@@ -1845,7 +1860,7 @@
         <v>147</v>
       </c>
       <c r="F49" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50">
@@ -1865,7 +1880,7 @@
         <v>143</v>
       </c>
       <c r="F50" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51">
@@ -1885,7 +1900,7 @@
         <v>147</v>
       </c>
       <c r="F51" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52">
@@ -1905,7 +1920,7 @@
         <v>190</v>
       </c>
       <c r="F52" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53">
@@ -1925,7 +1940,7 @@
         <v>147</v>
       </c>
       <c r="F53" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54">
@@ -1945,7 +1960,7 @@
         <v>143</v>
       </c>
       <c r="F54" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55">
@@ -1965,7 +1980,7 @@
         <v>147</v>
       </c>
       <c r="F55" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56">
@@ -1985,7 +2000,7 @@
         <v>191</v>
       </c>
       <c r="F56" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57">
@@ -2005,7 +2020,7 @@
         <v>64</v>
       </c>
       <c r="F57" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58">
@@ -2025,7 +2040,7 @@
         <v>192</v>
       </c>
       <c r="F58" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59">
@@ -2065,7 +2080,7 @@
         <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>263</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61">
@@ -2085,7 +2100,7 @@
         <v>64</v>
       </c>
       <c r="F61" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62">
@@ -2105,7 +2120,7 @@
         <v>192</v>
       </c>
       <c r="F62" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63">
@@ -2123,6 +2138,9 @@
       </c>
       <c r="E63" t="s">
         <v>194</v>
+      </c>
+      <c r="F63" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="64">

</xml_diff>